<commit_message>
Fixed issues in test data and accounting rule filters
</commit_message>
<xml_diff>
--- a/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata_SGN.xlsx
+++ b/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata_SGN.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="146">
   <si>
     <t>UseCase</t>
   </si>
@@ -325,9 +325,6 @@
   </si>
   <si>
     <t>Spring Hermann</t>
-  </si>
-  <si>
-    <t>2339-M</t>
   </si>
   <si>
     <t xml:space="preserve">Start und Landung Doppelsitzer Club-Segelflugzeug auf Homebase mit einem zweiten Piloten oder Passagier / Schlepp mit Club-eigenem Schleppflugzeug EXW und Turbo gebrauch </t>
@@ -480,6 +477,15 @@
   </si>
   <si>
     <t>1622-S</t>
+  </si>
+  <si>
+    <t>1593</t>
+  </si>
+  <si>
+    <t>EXW-FS-U</t>
+  </si>
+  <si>
+    <t>6203</t>
   </si>
 </sst>
 </file>
@@ -1309,9 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL10" sqref="AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1405,7 @@
         <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>20</v>
@@ -1551,7 +1557,7 @@
         <v>80</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J2" s="1">
         <v>1</v>
@@ -1611,7 +1617,7 @@
         <v>83</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH2" s="1">
         <v>0</v>
@@ -1664,7 +1670,7 @@
         <v>87</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
@@ -1724,7 +1730,7 @@
         <v>83</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH3" s="1">
         <v>0</v>
@@ -1777,7 +1783,7 @@
         <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
@@ -1786,7 +1792,7 @@
         <v>92</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>93</v>
@@ -1837,16 +1843,16 @@
         <v>92</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AH4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI4" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AJ4" s="1">
         <v>20</v>
@@ -1893,7 +1899,7 @@
         <v>70</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
@@ -1947,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="AD5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE5" s="1" t="s">
         <v>97</v>
@@ -1956,7 +1962,7 @@
         <v>99</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AH5" s="1">
         <v>0</v>
@@ -1971,30 +1977,21 @@
         <v>67</v>
       </c>
       <c r="AL5" s="5" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="AM5" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AN5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AO5" s="5" t="s">
-        <v>86</v>
+      <c r="AO5" s="5">
+        <v>6203</v>
       </c>
       <c r="AP5" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR5" s="5">
-        <v>6203</v>
-      </c>
-      <c r="AS5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT5" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2006,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>63</v>
@@ -2015,19 +2012,19 @@
         <v>81</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>98</v>
@@ -2048,10 +2045,10 @@
         <v>180</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>85</v>
@@ -2075,13 +2072,13 @@
         <v>4</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
@@ -2096,10 +2093,10 @@
         <v>67</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM6" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>67</v>
@@ -2131,31 +2128,31 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="J7" s="1">
         <v>3</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="P7" s="1">
         <v>60</v>
@@ -2176,7 +2173,7 @@
         <v>900</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AC7" s="1">
         <v>1</v>
@@ -2185,13 +2182,13 @@
         <v>3</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH7" s="1">
         <v>0</v>
@@ -2206,7 +2203,7 @@
         <v>67</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AM7" s="1">
         <v>15</v>
@@ -2232,7 +2229,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>63</v>
@@ -2241,19 +2238,19 @@
         <v>88</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="1">
-        <v>1</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P8" s="1">
         <v>61</v>
@@ -2271,7 +2268,7 @@
         <v>180</v>
       </c>
       <c r="U8">
-        <v>10</v>
+        <v>600</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>72</v>
@@ -2298,13 +2295,13 @@
         <v>4</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AH8" s="1">
         <v>0</v>
@@ -2319,19 +2316,19 @@
         <v>67</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="AM8" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AN8" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="AP8" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AQ8" s="1" t="s">
         <v>67</v>
@@ -2354,7 +2351,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>63</v>
@@ -2363,19 +2360,19 @@
         <v>81</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J9" s="1">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="P9" s="1">
         <v>60</v>
@@ -2396,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>85</v>
@@ -2420,13 +2417,13 @@
         <v>2</v>
       </c>
       <c r="AE9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF9" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AF9" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="AG9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH9" s="1">
         <v>0</v>
@@ -2458,19 +2455,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>63</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>64</v>
@@ -2479,10 +2476,10 @@
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="P10" s="1">
         <v>60</v>
@@ -2503,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>77</v>
@@ -2527,19 +2524,19 @@
         <v>2</v>
       </c>
       <c r="AE10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF10" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AF10" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="AG10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH10" s="1">
         <v>0</v>
       </c>
-      <c r="AI10" s="5">
-        <v>3144</v>
+      <c r="AI10" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="AJ10" s="1">
         <v>100</v>
@@ -2547,8 +2544,8 @@
       <c r="AK10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AL10" s="5">
-        <v>6200</v>
+      <c r="AL10" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="AM10" s="1">
         <v>1</v>
@@ -2565,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>63</v>
@@ -2574,19 +2571,19 @@
         <v>81</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J11" s="1">
         <v>1</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>98</v>
@@ -2601,16 +2598,16 @@
         <v>84</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="T11" s="1">
         <v>180</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>85</v>
@@ -2634,13 +2631,13 @@
         <v>3</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AH11" s="1">
         <v>0</v>
@@ -2655,19 +2652,19 @@
         <v>67</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AM11" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AO11" s="5" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="AP11" s="1">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AQ11" s="1" t="s">
         <v>67</v>
@@ -2678,7 +2675,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>73</v>
@@ -2693,7 +2690,7 @@
         <v>74</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J12" s="1">
         <v>1</v>
@@ -2702,7 +2699,7 @@
         <v>92</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>93</v>
@@ -2753,16 +2750,16 @@
         <v>92</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AH12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="5">
-        <v>6203</v>
+        <v>1</v>
+      </c>
+      <c r="AI12" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="AJ12" s="1">
         <v>20</v>
@@ -2794,7 +2791,7 @@
         <v>45</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>73</v>
@@ -2809,7 +2806,7 @@
         <v>74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J13" s="1">
         <v>1</v>
@@ -2818,7 +2815,7 @@
         <v>92</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>93</v>
@@ -2869,16 +2866,16 @@
         <v>92</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AH13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="5">
-        <v>2341</v>
+        <v>1</v>
+      </c>
+      <c r="AI13" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="AJ13" s="1">
         <v>20</v>
@@ -2886,8 +2883,8 @@
       <c r="AK13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AL13" s="5">
-        <v>6203</v>
+      <c r="AL13" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="AM13" s="1">
         <v>8</v>

</xml_diff>

<commit_message>
Close #75: Take NrOfLdgs value instead hard-coded 1 landing for the quantity Added LandingTaxOnStartLocationRule and VsfFeeOnStartLocationRule to catch nr of landings on start location Added more unit tests for motor flight testing and implemented master data feeder for xlsx files
</commit_message>
<xml_diff>
--- a/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata_SGN.xlsx
+++ b/src/FLS.Server.Tests/TestData/FlightInvoiceTestdata_SGN.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="146">
   <si>
     <t>UseCase</t>
   </si>
@@ -1315,9 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AL10" sqref="AL10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,10 +2030,10 @@
         <v>98</v>
       </c>
       <c r="P6" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>84</v>
@@ -2048,7 +2048,7 @@
         <v>300</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>85</v>
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="AD6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE6" s="1" t="s">
         <v>102</v>
@@ -2078,45 +2078,36 @@
         <v>124</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AH6" s="1">
         <v>0</v>
       </c>
-      <c r="AI6" s="5">
-        <v>2341</v>
+      <c r="AI6" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="AJ6" s="1">
-        <v>180</v>
+        <v>5</v>
       </c>
       <c r="AK6" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AL6" s="5" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="AM6" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AO6" s="5" t="s">
-        <v>86</v>
+      <c r="AO6" s="5">
+        <v>6203</v>
       </c>
       <c r="AP6" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR6" s="5">
-        <v>6203</v>
-      </c>
-      <c r="AS6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AT6" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2589,10 +2580,10 @@
         <v>98</v>
       </c>
       <c r="P11" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>84</v>
@@ -2607,7 +2598,7 @@
         <v>180</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>85</v>
@@ -2628,7 +2619,7 @@
         <v>1</v>
       </c>
       <c r="AD11" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE11" s="1" t="s">
         <v>102</v>
@@ -2637,36 +2628,27 @@
         <v>124</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AH11" s="1">
         <v>0</v>
       </c>
-      <c r="AI11" s="5">
-        <v>2341</v>
+      <c r="AI11" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="AJ11" s="1">
-        <v>180</v>
+        <v>3</v>
       </c>
       <c r="AK11" s="1" t="s">
         <v>67</v>
       </c>
       <c r="AL11" s="5" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="AM11" s="1">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO11" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="AP11" s="1">
-        <v>25</v>
-      </c>
-      <c r="AQ11" s="1" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>